<commit_message>
bdd.php : fonction str2url
admin.php : fonction addSection et supprSection

sections.php : formulaire ajout de section + mise en page

utilisateurs.php : mise en page
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8666EDAE-89FA-4149-930F-417BC509E7C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE416A9-D6AC-4087-9791-5A4C9091DB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="fin_tâche" localSheetId="0">PlanningProjet!$F1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PlanningProjet!$4:$6</definedName>
     <definedName name="Semaine_Affichage">PlanningProjet!$E$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PlanningProjet!$B$1:$EY$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PlanningProjet!$B$1:$EY$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>Entrez le nom de la société dans la cellule B2.</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Header/footer</t>
   </si>
   <si>
-    <t>Publication article</t>
-  </si>
-  <si>
     <t>Archivage articles</t>
   </si>
   <si>
@@ -256,6 +253,15 @@
   </si>
   <si>
     <t>Publication automatique sur Facebook</t>
+  </si>
+  <si>
+    <t>Publication articles</t>
+  </si>
+  <si>
+    <t>Gestion rédacteur</t>
+  </si>
+  <si>
+    <t>Gestion relecteur</t>
   </si>
 </sst>
 </file>
@@ -1290,31 +1296,31 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20 % - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1372,7 +1378,59 @@
     <cellStyle name="Vérification" xfId="25" builtinId="23" customBuiltin="1"/>
     <cellStyle name="zTexteMasqué" xfId="3" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1520,15 +1578,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="lastColumn" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumn" dxfId="17"/>
+      <tableStyleElement type="lastColumn" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1943,11 +2001,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EY31"/>
+  <dimension ref="A1:EY33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CA12" sqref="CA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2036,244 +2094,244 @@
         <v>1</v>
       </c>
       <c r="B3" s="48"/>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="92">
+      <c r="D3" s="91"/>
+      <c r="E3" s="87">
         <v>43892</v>
       </c>
-      <c r="F3" s="92"/>
+      <c r="F3" s="87"/>
     </row>
     <row r="4" spans="1:155" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="87"/>
-      <c r="I4" s="89">
+      <c r="C4" s="88"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
+      <c r="I4" s="84">
         <f>I5</f>
         <v>43892</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="89">
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="84">
         <f>P5</f>
         <v>43899</v>
       </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="89">
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="84">
         <f>W5</f>
         <v>43906</v>
       </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="89">
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="86"/>
+      <c r="AD4" s="84">
         <f>AD5</f>
         <v>43913</v>
       </c>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="89">
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="85"/>
+      <c r="AG4" s="85"/>
+      <c r="AH4" s="85"/>
+      <c r="AI4" s="85"/>
+      <c r="AJ4" s="86"/>
+      <c r="AK4" s="84">
         <f>AK5</f>
         <v>43920</v>
       </c>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="90"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="89">
+      <c r="AL4" s="85"/>
+      <c r="AM4" s="85"/>
+      <c r="AN4" s="85"/>
+      <c r="AO4" s="85"/>
+      <c r="AP4" s="85"/>
+      <c r="AQ4" s="86"/>
+      <c r="AR4" s="84">
         <f>AR5</f>
         <v>43927</v>
       </c>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="89">
+      <c r="AS4" s="85"/>
+      <c r="AT4" s="85"/>
+      <c r="AU4" s="85"/>
+      <c r="AV4" s="85"/>
+      <c r="AW4" s="85"/>
+      <c r="AX4" s="86"/>
+      <c r="AY4" s="84">
         <f>AY5</f>
         <v>43934</v>
       </c>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="89">
+      <c r="AZ4" s="85"/>
+      <c r="BA4" s="85"/>
+      <c r="BB4" s="85"/>
+      <c r="BC4" s="85"/>
+      <c r="BD4" s="85"/>
+      <c r="BE4" s="86"/>
+      <c r="BF4" s="84">
         <f>BF5</f>
         <v>43941</v>
       </c>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="90"/>
-      <c r="BI4" s="90"/>
-      <c r="BJ4" s="90"/>
-      <c r="BK4" s="90"/>
-      <c r="BL4" s="91"/>
-      <c r="BM4" s="89">
+      <c r="BG4" s="85"/>
+      <c r="BH4" s="85"/>
+      <c r="BI4" s="85"/>
+      <c r="BJ4" s="85"/>
+      <c r="BK4" s="85"/>
+      <c r="BL4" s="86"/>
+      <c r="BM4" s="84">
         <f>BM5</f>
         <v>43948</v>
       </c>
-      <c r="BN4" s="90"/>
-      <c r="BO4" s="90"/>
-      <c r="BP4" s="90"/>
-      <c r="BQ4" s="90"/>
-      <c r="BR4" s="90"/>
-      <c r="BS4" s="91"/>
-      <c r="BT4" s="89">
+      <c r="BN4" s="85"/>
+      <c r="BO4" s="85"/>
+      <c r="BP4" s="85"/>
+      <c r="BQ4" s="85"/>
+      <c r="BR4" s="85"/>
+      <c r="BS4" s="86"/>
+      <c r="BT4" s="84">
         <f>BT5</f>
         <v>43955</v>
       </c>
-      <c r="BU4" s="90"/>
-      <c r="BV4" s="90"/>
-      <c r="BW4" s="90"/>
-      <c r="BX4" s="90"/>
-      <c r="BY4" s="90"/>
-      <c r="BZ4" s="91"/>
-      <c r="CA4" s="89">
+      <c r="BU4" s="85"/>
+      <c r="BV4" s="85"/>
+      <c r="BW4" s="85"/>
+      <c r="BX4" s="85"/>
+      <c r="BY4" s="85"/>
+      <c r="BZ4" s="86"/>
+      <c r="CA4" s="84">
         <f>CA5</f>
         <v>43962</v>
       </c>
-      <c r="CB4" s="90"/>
-      <c r="CC4" s="90"/>
-      <c r="CD4" s="90"/>
-      <c r="CE4" s="90"/>
-      <c r="CF4" s="90"/>
-      <c r="CG4" s="91"/>
-      <c r="CH4" s="89">
+      <c r="CB4" s="85"/>
+      <c r="CC4" s="85"/>
+      <c r="CD4" s="85"/>
+      <c r="CE4" s="85"/>
+      <c r="CF4" s="85"/>
+      <c r="CG4" s="86"/>
+      <c r="CH4" s="84">
         <f>CH5</f>
         <v>43969</v>
       </c>
-      <c r="CI4" s="90"/>
-      <c r="CJ4" s="90"/>
-      <c r="CK4" s="90"/>
-      <c r="CL4" s="90"/>
-      <c r="CM4" s="90"/>
-      <c r="CN4" s="91"/>
-      <c r="CO4" s="89">
+      <c r="CI4" s="85"/>
+      <c r="CJ4" s="85"/>
+      <c r="CK4" s="85"/>
+      <c r="CL4" s="85"/>
+      <c r="CM4" s="85"/>
+      <c r="CN4" s="86"/>
+      <c r="CO4" s="84">
         <f>CO5</f>
         <v>43976</v>
       </c>
-      <c r="CP4" s="90"/>
-      <c r="CQ4" s="90"/>
-      <c r="CR4" s="90"/>
-      <c r="CS4" s="90"/>
-      <c r="CT4" s="90"/>
-      <c r="CU4" s="91"/>
-      <c r="CV4" s="89">
+      <c r="CP4" s="85"/>
+      <c r="CQ4" s="85"/>
+      <c r="CR4" s="85"/>
+      <c r="CS4" s="85"/>
+      <c r="CT4" s="85"/>
+      <c r="CU4" s="86"/>
+      <c r="CV4" s="84">
         <f>CV5</f>
         <v>43983</v>
       </c>
-      <c r="CW4" s="90"/>
-      <c r="CX4" s="90"/>
-      <c r="CY4" s="90"/>
-      <c r="CZ4" s="90"/>
-      <c r="DA4" s="90"/>
-      <c r="DB4" s="91"/>
-      <c r="DC4" s="89">
+      <c r="CW4" s="85"/>
+      <c r="CX4" s="85"/>
+      <c r="CY4" s="85"/>
+      <c r="CZ4" s="85"/>
+      <c r="DA4" s="85"/>
+      <c r="DB4" s="86"/>
+      <c r="DC4" s="84">
         <f>DC5</f>
         <v>43990</v>
       </c>
-      <c r="DD4" s="90"/>
-      <c r="DE4" s="90"/>
-      <c r="DF4" s="90"/>
-      <c r="DG4" s="90"/>
-      <c r="DH4" s="90"/>
-      <c r="DI4" s="91"/>
-      <c r="DJ4" s="89">
+      <c r="DD4" s="85"/>
+      <c r="DE4" s="85"/>
+      <c r="DF4" s="85"/>
+      <c r="DG4" s="85"/>
+      <c r="DH4" s="85"/>
+      <c r="DI4" s="86"/>
+      <c r="DJ4" s="84">
         <f>DJ5</f>
         <v>43997</v>
       </c>
-      <c r="DK4" s="90"/>
-      <c r="DL4" s="90"/>
-      <c r="DM4" s="90"/>
-      <c r="DN4" s="90"/>
-      <c r="DO4" s="90"/>
-      <c r="DP4" s="91"/>
-      <c r="DQ4" s="89">
+      <c r="DK4" s="85"/>
+      <c r="DL4" s="85"/>
+      <c r="DM4" s="85"/>
+      <c r="DN4" s="85"/>
+      <c r="DO4" s="85"/>
+      <c r="DP4" s="86"/>
+      <c r="DQ4" s="84">
         <f>DQ5</f>
         <v>44004</v>
       </c>
-      <c r="DR4" s="90"/>
-      <c r="DS4" s="90"/>
-      <c r="DT4" s="90"/>
-      <c r="DU4" s="90"/>
-      <c r="DV4" s="90"/>
-      <c r="DW4" s="91"/>
-      <c r="DX4" s="89">
+      <c r="DR4" s="85"/>
+      <c r="DS4" s="85"/>
+      <c r="DT4" s="85"/>
+      <c r="DU4" s="85"/>
+      <c r="DV4" s="85"/>
+      <c r="DW4" s="86"/>
+      <c r="DX4" s="84">
         <f>DX5</f>
         <v>44011</v>
       </c>
-      <c r="DY4" s="90"/>
-      <c r="DZ4" s="90"/>
-      <c r="EA4" s="90"/>
-      <c r="EB4" s="90"/>
-      <c r="EC4" s="90"/>
-      <c r="ED4" s="91"/>
-      <c r="EE4" s="89">
+      <c r="DY4" s="85"/>
+      <c r="DZ4" s="85"/>
+      <c r="EA4" s="85"/>
+      <c r="EB4" s="85"/>
+      <c r="EC4" s="85"/>
+      <c r="ED4" s="86"/>
+      <c r="EE4" s="84">
         <f>EE5</f>
         <v>44018</v>
       </c>
-      <c r="EF4" s="90"/>
-      <c r="EG4" s="90"/>
-      <c r="EH4" s="90"/>
-      <c r="EI4" s="90"/>
-      <c r="EJ4" s="90"/>
-      <c r="EK4" s="91"/>
-      <c r="EL4" s="89">
+      <c r="EF4" s="85"/>
+      <c r="EG4" s="85"/>
+      <c r="EH4" s="85"/>
+      <c r="EI4" s="85"/>
+      <c r="EJ4" s="85"/>
+      <c r="EK4" s="86"/>
+      <c r="EL4" s="84">
         <f>EL5</f>
         <v>44025</v>
       </c>
-      <c r="EM4" s="90"/>
-      <c r="EN4" s="90"/>
-      <c r="EO4" s="90"/>
-      <c r="EP4" s="90"/>
-      <c r="EQ4" s="90"/>
-      <c r="ER4" s="91"/>
-      <c r="ES4" s="89">
+      <c r="EM4" s="85"/>
+      <c r="EN4" s="85"/>
+      <c r="EO4" s="85"/>
+      <c r="EP4" s="85"/>
+      <c r="EQ4" s="85"/>
+      <c r="ER4" s="86"/>
+      <c r="ES4" s="84">
         <f>ES5</f>
         <v>44032</v>
       </c>
-      <c r="ET4" s="90"/>
-      <c r="EU4" s="90"/>
-      <c r="EV4" s="90"/>
-      <c r="EW4" s="90"/>
-      <c r="EX4" s="90"/>
-      <c r="EY4" s="91"/>
+      <c r="ET4" s="85"/>
+      <c r="EU4" s="85"/>
+      <c r="EV4" s="85"/>
+      <c r="EW4" s="85"/>
+      <c r="EX4" s="85"/>
+      <c r="EY4" s="86"/>
     </row>
     <row r="5" spans="1:155" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
       <c r="I5" s="80">
         <v>43892</v>
       </c>
@@ -3481,7 +3539,7 @@
       <c r="C7" s="45"/>
       <c r="E7"/>
       <c r="H7" t="e">
-        <f t="shared" ref="H7:H28" ca="1" si="72">IF(OR(ISBLANK(_xlfn.SINGLE(début_tâche)),ISBLANK(_xlfn.SINGLE(fin_tâche))),"",_xlfn.SINGLE(fin_tâche)-_xlfn.SINGLE(début_tâche)+1)</f>
+        <f t="shared" ref="H7:H30" ca="1" si="72">IF(OR(ISBLANK(_xlfn.SINGLE(début_tâche)),ISBLANK(_xlfn.SINGLE(fin_tâche))),"",_xlfn.SINGLE(fin_tâche)-_xlfn.SINGLE(début_tâche)+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="I7" s="29"/>
@@ -4821,7 +4879,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="21"/>
@@ -5153,19 +5211,19 @@
     <row r="17" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="41"/>
       <c r="B17" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="22">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E17" s="74">
         <v>43911</v>
       </c>
       <c r="F17" s="74">
-        <v>43951</v>
+        <v>43971</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -5320,19 +5378,19 @@
     <row r="18" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="41"/>
       <c r="B18" s="60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E18" s="74">
-        <v>43941</v>
+        <v>43955</v>
       </c>
       <c r="F18" s="74">
-        <v>43966</v>
+        <v>43981</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
@@ -5487,7 +5545,7 @@
     <row r="19" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="41"/>
       <c r="B19" s="60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="54" t="s">
         <v>47</v>
@@ -5496,7 +5554,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="74">
-        <v>43952</v>
+        <v>43976</v>
       </c>
       <c r="F19" s="74">
         <v>43981</v>
@@ -5657,7 +5715,7 @@
     <row r="20" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="41"/>
       <c r="B20" s="60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="54" t="s">
         <v>47</v>
@@ -5666,10 +5724,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="74">
-        <v>43952</v>
+        <v>43981</v>
       </c>
       <c r="F20" s="74">
-        <v>43966</v>
+        <v>43997</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13" t="e">
@@ -5829,7 +5887,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="55"/>
       <c r="D21" s="24"/>
@@ -5991,7 +6049,7 @@
     <row r="22" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="41"/>
       <c r="B22" s="61" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C22" s="56" t="s">
         <v>45</v>
@@ -6000,10 +6058,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="77">
-        <v>43927</v>
+        <v>43961</v>
       </c>
       <c r="F22" s="77">
-        <v>43957</v>
+        <v>43997</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13" t="e">
@@ -6161,7 +6219,7 @@
     <row r="23" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="41"/>
       <c r="B23" s="61" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C23" s="56" t="s">
         <v>45</v>
@@ -6170,10 +6228,10 @@
         <v>0</v>
       </c>
       <c r="E23" s="77">
-        <v>43931</v>
+        <v>43961</v>
       </c>
       <c r="F23" s="77">
-        <v>43957</v>
+        <v>43997</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13" t="e">
@@ -6331,7 +6389,7 @@
     <row r="24" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="41"/>
       <c r="B24" s="61" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" s="56" t="s">
         <v>45</v>
@@ -6340,10 +6398,10 @@
         <v>0</v>
       </c>
       <c r="E24" s="77">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="F24" s="77">
-        <v>43971</v>
+        <v>43981</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13" t="e">
@@ -6501,7 +6559,7 @@
     <row r="25" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="41"/>
       <c r="B25" s="61" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C25" s="56" t="s">
         <v>45</v>
@@ -6510,10 +6568,10 @@
         <v>0</v>
       </c>
       <c r="E25" s="77">
-        <v>43972</v>
+        <v>43961</v>
       </c>
       <c r="F25" s="77">
-        <v>43992</v>
+        <v>43971</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13" t="e">
@@ -6668,20 +6726,22 @@
       <c r="EX25" s="29"/>
       <c r="EY25" s="29"/>
     </row>
-    <row r="26" spans="1:155" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="41"/>
       <c r="B26" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="56"/>
+        <v>50</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="D26" s="25">
         <v>0</v>
       </c>
-      <c r="E26" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="77" t="s">
-        <v>18</v>
+      <c r="E26" s="77">
+        <v>43966</v>
+      </c>
+      <c r="F26" s="77">
+        <v>43981</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="13" t="e">
@@ -6837,14 +6897,22 @@
       <c r="EY26" s="29"/>
     </row>
     <row r="27" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="62"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="25">
+        <v>0</v>
+      </c>
+      <c r="E27" s="77">
+        <v>43972</v>
+      </c>
+      <c r="F27" s="77">
+        <v>43992</v>
+      </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13" t="e">
         <f t="shared" ca="1" si="72"/>
@@ -6998,189 +7066,517 @@
       <c r="EX27" s="29"/>
       <c r="EY27" s="29"/>
     </row>
-    <row r="28" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28" t="e">
+    <row r="28" spans="1:155" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="41"/>
+      <c r="B28" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="56"/>
+      <c r="D28" s="25">
+        <v>0</v>
+      </c>
+      <c r="E28" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13" t="e">
         <f t="shared" ca="1" si="72"/>
         <v>#NAME?</v>
       </c>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="31"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
-      <c r="X28" s="31"/>
-      <c r="Y28" s="31"/>
-      <c r="Z28" s="31"/>
-      <c r="AA28" s="31"/>
-      <c r="AB28" s="31"/>
-      <c r="AC28" s="31"/>
-      <c r="AD28" s="31"/>
-      <c r="AE28" s="31"/>
-      <c r="AF28" s="31"/>
-      <c r="AG28" s="31"/>
-      <c r="AH28" s="31"/>
-      <c r="AI28" s="31"/>
-      <c r="AJ28" s="31"/>
-      <c r="AK28" s="31"/>
-      <c r="AL28" s="31"/>
-      <c r="AM28" s="31"/>
-      <c r="AN28" s="31"/>
-      <c r="AO28" s="31"/>
-      <c r="AP28" s="31"/>
-      <c r="AQ28" s="31"/>
-      <c r="AR28" s="31"/>
-      <c r="AS28" s="31"/>
-      <c r="AT28" s="31"/>
-      <c r="AU28" s="31"/>
-      <c r="AV28" s="31"/>
-      <c r="AW28" s="31"/>
-      <c r="AX28" s="31"/>
-      <c r="AY28" s="31"/>
-      <c r="AZ28" s="31"/>
-      <c r="BA28" s="31"/>
-      <c r="BB28" s="31"/>
-      <c r="BC28" s="31"/>
-      <c r="BD28" s="31"/>
-      <c r="BE28" s="31"/>
-      <c r="BF28" s="31"/>
-      <c r="BG28" s="31"/>
-      <c r="BH28" s="31"/>
-      <c r="BI28" s="31"/>
-      <c r="BJ28" s="31"/>
-      <c r="BK28" s="31"/>
-      <c r="BL28" s="31"/>
-      <c r="BM28" s="31"/>
-      <c r="BN28" s="31"/>
-      <c r="BO28" s="31"/>
-      <c r="BP28" s="31"/>
-      <c r="BQ28" s="31"/>
-      <c r="BR28" s="31"/>
-      <c r="BS28" s="31"/>
-      <c r="BT28" s="31"/>
-      <c r="BU28" s="31"/>
-      <c r="BV28" s="31"/>
-      <c r="BW28" s="31"/>
-      <c r="BX28" s="31"/>
-      <c r="BY28" s="31"/>
-      <c r="BZ28" s="31"/>
-      <c r="CA28" s="31"/>
-      <c r="CB28" s="31"/>
-      <c r="CC28" s="31"/>
-      <c r="CD28" s="31"/>
-      <c r="CE28" s="31"/>
-      <c r="CF28" s="31"/>
-      <c r="CG28" s="31"/>
-      <c r="CH28" s="31"/>
-      <c r="CI28" s="31"/>
-      <c r="CJ28" s="31"/>
-      <c r="CK28" s="31"/>
-      <c r="CL28" s="31"/>
-      <c r="CM28" s="31"/>
-      <c r="CN28" s="31"/>
-      <c r="CO28" s="31"/>
-      <c r="CP28" s="31"/>
-      <c r="CQ28" s="31"/>
-      <c r="CR28" s="31"/>
-      <c r="CS28" s="31"/>
-      <c r="CT28" s="31"/>
-      <c r="CU28" s="31"/>
-      <c r="CV28" s="31"/>
-      <c r="CW28" s="31"/>
-      <c r="CX28" s="31"/>
-      <c r="CY28" s="31"/>
-      <c r="CZ28" s="31"/>
-      <c r="DA28" s="31"/>
-      <c r="DB28" s="31"/>
-      <c r="DC28" s="31"/>
-      <c r="DD28" s="31"/>
-      <c r="DE28" s="31"/>
-      <c r="DF28" s="31"/>
-      <c r="DG28" s="31"/>
-      <c r="DH28" s="31"/>
-      <c r="DI28" s="31"/>
-      <c r="DJ28" s="31"/>
-      <c r="DK28" s="31"/>
-      <c r="DL28" s="31"/>
-      <c r="DM28" s="31"/>
-      <c r="DN28" s="31"/>
-      <c r="DO28" s="31"/>
-      <c r="DP28" s="31"/>
-      <c r="DQ28" s="31"/>
-      <c r="DR28" s="31"/>
-      <c r="DS28" s="31"/>
-      <c r="DT28" s="31"/>
-      <c r="DU28" s="31"/>
-      <c r="DV28" s="31"/>
-      <c r="DW28" s="31"/>
-      <c r="DX28" s="31"/>
-      <c r="DY28" s="31"/>
-      <c r="DZ28" s="31"/>
-      <c r="EA28" s="31"/>
-      <c r="EB28" s="31"/>
-      <c r="EC28" s="31"/>
-      <c r="ED28" s="31"/>
-      <c r="EE28" s="31"/>
-      <c r="EF28" s="31"/>
-      <c r="EG28" s="31"/>
-      <c r="EH28" s="31"/>
-      <c r="EI28" s="31"/>
-      <c r="EJ28" s="31"/>
-      <c r="EK28" s="31"/>
-      <c r="EL28" s="31"/>
-      <c r="EM28" s="31"/>
-      <c r="EN28" s="31"/>
-      <c r="EO28" s="31"/>
-      <c r="EP28" s="31"/>
-      <c r="EQ28" s="31"/>
-      <c r="ER28" s="31"/>
-      <c r="ES28" s="31"/>
-      <c r="ET28" s="31"/>
-      <c r="EU28" s="31"/>
-      <c r="EV28" s="31"/>
-      <c r="EW28" s="31"/>
-      <c r="EX28" s="31"/>
-      <c r="EY28" s="31"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+      <c r="AA28" s="29"/>
+      <c r="AB28" s="29"/>
+      <c r="AC28" s="29"/>
+      <c r="AD28" s="29"/>
+      <c r="AE28" s="29"/>
+      <c r="AF28" s="29"/>
+      <c r="AG28" s="29"/>
+      <c r="AH28" s="29"/>
+      <c r="AI28" s="29"/>
+      <c r="AJ28" s="29"/>
+      <c r="AK28" s="29"/>
+      <c r="AL28" s="29"/>
+      <c r="AM28" s="29"/>
+      <c r="AN28" s="29"/>
+      <c r="AO28" s="29"/>
+      <c r="AP28" s="29"/>
+      <c r="AQ28" s="29"/>
+      <c r="AR28" s="29"/>
+      <c r="AS28" s="29"/>
+      <c r="AT28" s="29"/>
+      <c r="AU28" s="29"/>
+      <c r="AV28" s="29"/>
+      <c r="AW28" s="29"/>
+      <c r="AX28" s="29"/>
+      <c r="AY28" s="29"/>
+      <c r="AZ28" s="29"/>
+      <c r="BA28" s="29"/>
+      <c r="BB28" s="29"/>
+      <c r="BC28" s="29"/>
+      <c r="BD28" s="29"/>
+      <c r="BE28" s="29"/>
+      <c r="BF28" s="29"/>
+      <c r="BG28" s="29"/>
+      <c r="BH28" s="29"/>
+      <c r="BI28" s="29"/>
+      <c r="BJ28" s="29"/>
+      <c r="BK28" s="29"/>
+      <c r="BL28" s="29"/>
+      <c r="BM28" s="29"/>
+      <c r="BN28" s="29"/>
+      <c r="BO28" s="29"/>
+      <c r="BP28" s="29"/>
+      <c r="BQ28" s="29"/>
+      <c r="BR28" s="29"/>
+      <c r="BS28" s="29"/>
+      <c r="BT28" s="29"/>
+      <c r="BU28" s="29"/>
+      <c r="BV28" s="29"/>
+      <c r="BW28" s="29"/>
+      <c r="BX28" s="29"/>
+      <c r="BY28" s="29"/>
+      <c r="BZ28" s="29"/>
+      <c r="CA28" s="29"/>
+      <c r="CB28" s="29"/>
+      <c r="CC28" s="29"/>
+      <c r="CD28" s="29"/>
+      <c r="CE28" s="29"/>
+      <c r="CF28" s="29"/>
+      <c r="CG28" s="29"/>
+      <c r="CH28" s="29"/>
+      <c r="CI28" s="29"/>
+      <c r="CJ28" s="29"/>
+      <c r="CK28" s="29"/>
+      <c r="CL28" s="29"/>
+      <c r="CM28" s="29"/>
+      <c r="CN28" s="29"/>
+      <c r="CO28" s="29"/>
+      <c r="CP28" s="29"/>
+      <c r="CQ28" s="29"/>
+      <c r="CR28" s="29"/>
+      <c r="CS28" s="29"/>
+      <c r="CT28" s="29"/>
+      <c r="CU28" s="29"/>
+      <c r="CV28" s="29"/>
+      <c r="CW28" s="29"/>
+      <c r="CX28" s="29"/>
+      <c r="CY28" s="29"/>
+      <c r="CZ28" s="29"/>
+      <c r="DA28" s="29"/>
+      <c r="DB28" s="29"/>
+      <c r="DC28" s="29"/>
+      <c r="DD28" s="29"/>
+      <c r="DE28" s="29"/>
+      <c r="DF28" s="29"/>
+      <c r="DG28" s="29"/>
+      <c r="DH28" s="29"/>
+      <c r="DI28" s="29"/>
+      <c r="DJ28" s="29"/>
+      <c r="DK28" s="29"/>
+      <c r="DL28" s="29"/>
+      <c r="DM28" s="29"/>
+      <c r="DN28" s="29"/>
+      <c r="DO28" s="29"/>
+      <c r="DP28" s="29"/>
+      <c r="DQ28" s="29"/>
+      <c r="DR28" s="29"/>
+      <c r="DS28" s="29"/>
+      <c r="DT28" s="29"/>
+      <c r="DU28" s="29"/>
+      <c r="DV28" s="29"/>
+      <c r="DW28" s="29"/>
+      <c r="DX28" s="29"/>
+      <c r="DY28" s="29"/>
+      <c r="DZ28" s="29"/>
+      <c r="EA28" s="29"/>
+      <c r="EB28" s="29"/>
+      <c r="EC28" s="29"/>
+      <c r="ED28" s="29"/>
+      <c r="EE28" s="29"/>
+      <c r="EF28" s="29"/>
+      <c r="EG28" s="29"/>
+      <c r="EH28" s="29"/>
+      <c r="EI28" s="29"/>
+      <c r="EJ28" s="29"/>
+      <c r="EK28" s="29"/>
+      <c r="EL28" s="29"/>
+      <c r="EM28" s="29"/>
+      <c r="EN28" s="29"/>
+      <c r="EO28" s="29"/>
+      <c r="EP28" s="29"/>
+      <c r="EQ28" s="29"/>
+      <c r="ER28" s="29"/>
+      <c r="ES28" s="29"/>
+      <c r="ET28" s="29"/>
+      <c r="EU28" s="29"/>
+      <c r="EV28" s="29"/>
+      <c r="EW28" s="29"/>
+      <c r="EX28" s="29"/>
+      <c r="EY28" s="29"/>
     </row>
-    <row r="29" spans="1:155" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G29" s="6"/>
+    <row r="29" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="62"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13" t="e">
+        <f t="shared" ca="1" si="72"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
+      <c r="AA29" s="29"/>
+      <c r="AB29" s="29"/>
+      <c r="AC29" s="29"/>
+      <c r="AD29" s="29"/>
+      <c r="AE29" s="29"/>
+      <c r="AF29" s="29"/>
+      <c r="AG29" s="29"/>
+      <c r="AH29" s="29"/>
+      <c r="AI29" s="29"/>
+      <c r="AJ29" s="29"/>
+      <c r="AK29" s="29"/>
+      <c r="AL29" s="29"/>
+      <c r="AM29" s="29"/>
+      <c r="AN29" s="29"/>
+      <c r="AO29" s="29"/>
+      <c r="AP29" s="29"/>
+      <c r="AQ29" s="29"/>
+      <c r="AR29" s="29"/>
+      <c r="AS29" s="29"/>
+      <c r="AT29" s="29"/>
+      <c r="AU29" s="29"/>
+      <c r="AV29" s="29"/>
+      <c r="AW29" s="29"/>
+      <c r="AX29" s="29"/>
+      <c r="AY29" s="29"/>
+      <c r="AZ29" s="29"/>
+      <c r="BA29" s="29"/>
+      <c r="BB29" s="29"/>
+      <c r="BC29" s="29"/>
+      <c r="BD29" s="29"/>
+      <c r="BE29" s="29"/>
+      <c r="BF29" s="29"/>
+      <c r="BG29" s="29"/>
+      <c r="BH29" s="29"/>
+      <c r="BI29" s="29"/>
+      <c r="BJ29" s="29"/>
+      <c r="BK29" s="29"/>
+      <c r="BL29" s="29"/>
+      <c r="BM29" s="29"/>
+      <c r="BN29" s="29"/>
+      <c r="BO29" s="29"/>
+      <c r="BP29" s="29"/>
+      <c r="BQ29" s="29"/>
+      <c r="BR29" s="29"/>
+      <c r="BS29" s="29"/>
+      <c r="BT29" s="29"/>
+      <c r="BU29" s="29"/>
+      <c r="BV29" s="29"/>
+      <c r="BW29" s="29"/>
+      <c r="BX29" s="29"/>
+      <c r="BY29" s="29"/>
+      <c r="BZ29" s="29"/>
+      <c r="CA29" s="29"/>
+      <c r="CB29" s="29"/>
+      <c r="CC29" s="29"/>
+      <c r="CD29" s="29"/>
+      <c r="CE29" s="29"/>
+      <c r="CF29" s="29"/>
+      <c r="CG29" s="29"/>
+      <c r="CH29" s="29"/>
+      <c r="CI29" s="29"/>
+      <c r="CJ29" s="29"/>
+      <c r="CK29" s="29"/>
+      <c r="CL29" s="29"/>
+      <c r="CM29" s="29"/>
+      <c r="CN29" s="29"/>
+      <c r="CO29" s="29"/>
+      <c r="CP29" s="29"/>
+      <c r="CQ29" s="29"/>
+      <c r="CR29" s="29"/>
+      <c r="CS29" s="29"/>
+      <c r="CT29" s="29"/>
+      <c r="CU29" s="29"/>
+      <c r="CV29" s="29"/>
+      <c r="CW29" s="29"/>
+      <c r="CX29" s="29"/>
+      <c r="CY29" s="29"/>
+      <c r="CZ29" s="29"/>
+      <c r="DA29" s="29"/>
+      <c r="DB29" s="29"/>
+      <c r="DC29" s="29"/>
+      <c r="DD29" s="29"/>
+      <c r="DE29" s="29"/>
+      <c r="DF29" s="29"/>
+      <c r="DG29" s="29"/>
+      <c r="DH29" s="29"/>
+      <c r="DI29" s="29"/>
+      <c r="DJ29" s="29"/>
+      <c r="DK29" s="29"/>
+      <c r="DL29" s="29"/>
+      <c r="DM29" s="29"/>
+      <c r="DN29" s="29"/>
+      <c r="DO29" s="29"/>
+      <c r="DP29" s="29"/>
+      <c r="DQ29" s="29"/>
+      <c r="DR29" s="29"/>
+      <c r="DS29" s="29"/>
+      <c r="DT29" s="29"/>
+      <c r="DU29" s="29"/>
+      <c r="DV29" s="29"/>
+      <c r="DW29" s="29"/>
+      <c r="DX29" s="29"/>
+      <c r="DY29" s="29"/>
+      <c r="DZ29" s="29"/>
+      <c r="EA29" s="29"/>
+      <c r="EB29" s="29"/>
+      <c r="EC29" s="29"/>
+      <c r="ED29" s="29"/>
+      <c r="EE29" s="29"/>
+      <c r="EF29" s="29"/>
+      <c r="EG29" s="29"/>
+      <c r="EH29" s="29"/>
+      <c r="EI29" s="29"/>
+      <c r="EJ29" s="29"/>
+      <c r="EK29" s="29"/>
+      <c r="EL29" s="29"/>
+      <c r="EM29" s="29"/>
+      <c r="EN29" s="29"/>
+      <c r="EO29" s="29"/>
+      <c r="EP29" s="29"/>
+      <c r="EQ29" s="29"/>
+      <c r="ER29" s="29"/>
+      <c r="ES29" s="29"/>
+      <c r="ET29" s="29"/>
+      <c r="EU29" s="29"/>
+      <c r="EV29" s="29"/>
+      <c r="EW29" s="29"/>
+      <c r="EX29" s="29"/>
+      <c r="EY29" s="29"/>
     </row>
-    <row r="30" spans="1:155" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="10"/>
-      <c r="F30" s="43"/>
+    <row r="30" spans="1:155" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="65"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28" t="e">
+        <f t="shared" ca="1" si="72"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="31"/>
+      <c r="AA30" s="31"/>
+      <c r="AB30" s="31"/>
+      <c r="AC30" s="31"/>
+      <c r="AD30" s="31"/>
+      <c r="AE30" s="31"/>
+      <c r="AF30" s="31"/>
+      <c r="AG30" s="31"/>
+      <c r="AH30" s="31"/>
+      <c r="AI30" s="31"/>
+      <c r="AJ30" s="31"/>
+      <c r="AK30" s="31"/>
+      <c r="AL30" s="31"/>
+      <c r="AM30" s="31"/>
+      <c r="AN30" s="31"/>
+      <c r="AO30" s="31"/>
+      <c r="AP30" s="31"/>
+      <c r="AQ30" s="31"/>
+      <c r="AR30" s="31"/>
+      <c r="AS30" s="31"/>
+      <c r="AT30" s="31"/>
+      <c r="AU30" s="31"/>
+      <c r="AV30" s="31"/>
+      <c r="AW30" s="31"/>
+      <c r="AX30" s="31"/>
+      <c r="AY30" s="31"/>
+      <c r="AZ30" s="31"/>
+      <c r="BA30" s="31"/>
+      <c r="BB30" s="31"/>
+      <c r="BC30" s="31"/>
+      <c r="BD30" s="31"/>
+      <c r="BE30" s="31"/>
+      <c r="BF30" s="31"/>
+      <c r="BG30" s="31"/>
+      <c r="BH30" s="31"/>
+      <c r="BI30" s="31"/>
+      <c r="BJ30" s="31"/>
+      <c r="BK30" s="31"/>
+      <c r="BL30" s="31"/>
+      <c r="BM30" s="31"/>
+      <c r="BN30" s="31"/>
+      <c r="BO30" s="31"/>
+      <c r="BP30" s="31"/>
+      <c r="BQ30" s="31"/>
+      <c r="BR30" s="31"/>
+      <c r="BS30" s="31"/>
+      <c r="BT30" s="31"/>
+      <c r="BU30" s="31"/>
+      <c r="BV30" s="31"/>
+      <c r="BW30" s="31"/>
+      <c r="BX30" s="31"/>
+      <c r="BY30" s="31"/>
+      <c r="BZ30" s="31"/>
+      <c r="CA30" s="31"/>
+      <c r="CB30" s="31"/>
+      <c r="CC30" s="31"/>
+      <c r="CD30" s="31"/>
+      <c r="CE30" s="31"/>
+      <c r="CF30" s="31"/>
+      <c r="CG30" s="31"/>
+      <c r="CH30" s="31"/>
+      <c r="CI30" s="31"/>
+      <c r="CJ30" s="31"/>
+      <c r="CK30" s="31"/>
+      <c r="CL30" s="31"/>
+      <c r="CM30" s="31"/>
+      <c r="CN30" s="31"/>
+      <c r="CO30" s="31"/>
+      <c r="CP30" s="31"/>
+      <c r="CQ30" s="31"/>
+      <c r="CR30" s="31"/>
+      <c r="CS30" s="31"/>
+      <c r="CT30" s="31"/>
+      <c r="CU30" s="31"/>
+      <c r="CV30" s="31"/>
+      <c r="CW30" s="31"/>
+      <c r="CX30" s="31"/>
+      <c r="CY30" s="31"/>
+      <c r="CZ30" s="31"/>
+      <c r="DA30" s="31"/>
+      <c r="DB30" s="31"/>
+      <c r="DC30" s="31"/>
+      <c r="DD30" s="31"/>
+      <c r="DE30" s="31"/>
+      <c r="DF30" s="31"/>
+      <c r="DG30" s="31"/>
+      <c r="DH30" s="31"/>
+      <c r="DI30" s="31"/>
+      <c r="DJ30" s="31"/>
+      <c r="DK30" s="31"/>
+      <c r="DL30" s="31"/>
+      <c r="DM30" s="31"/>
+      <c r="DN30" s="31"/>
+      <c r="DO30" s="31"/>
+      <c r="DP30" s="31"/>
+      <c r="DQ30" s="31"/>
+      <c r="DR30" s="31"/>
+      <c r="DS30" s="31"/>
+      <c r="DT30" s="31"/>
+      <c r="DU30" s="31"/>
+      <c r="DV30" s="31"/>
+      <c r="DW30" s="31"/>
+      <c r="DX30" s="31"/>
+      <c r="DY30" s="31"/>
+      <c r="DZ30" s="31"/>
+      <c r="EA30" s="31"/>
+      <c r="EB30" s="31"/>
+      <c r="EC30" s="31"/>
+      <c r="ED30" s="31"/>
+      <c r="EE30" s="31"/>
+      <c r="EF30" s="31"/>
+      <c r="EG30" s="31"/>
+      <c r="EH30" s="31"/>
+      <c r="EI30" s="31"/>
+      <c r="EJ30" s="31"/>
+      <c r="EK30" s="31"/>
+      <c r="EL30" s="31"/>
+      <c r="EM30" s="31"/>
+      <c r="EN30" s="31"/>
+      <c r="EO30" s="31"/>
+      <c r="EP30" s="31"/>
+      <c r="EQ30" s="31"/>
+      <c r="ER30" s="31"/>
+      <c r="ES30" s="31"/>
+      <c r="ET30" s="31"/>
+      <c r="EU30" s="31"/>
+      <c r="EV30" s="31"/>
+      <c r="EW30" s="31"/>
+      <c r="EX30" s="31"/>
+      <c r="EY30" s="31"/>
     </row>
     <row r="31" spans="1:155" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="11"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:155" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="10"/>
+      <c r="F32" s="43"/>
+    </row>
+    <row r="33" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
@@ -7195,14 +7591,16 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D27:D28 D7:D21">
-    <cfRule type="dataBar" priority="19">
+  <conditionalFormatting sqref="D7:D21 D24:D30">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7215,32 +7613,66 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:EY28">
-    <cfRule type="expression" dxfId="5" priority="38">
+  <conditionalFormatting sqref="I5:EY21 I24:EY30">
+    <cfRule type="expression" dxfId="11" priority="46">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:EY28">
-    <cfRule type="expression" dxfId="4" priority="32">
+  <conditionalFormatting sqref="I7:EY21 I24:EY30">
+    <cfRule type="expression" dxfId="10" priority="40">
       <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:EY11">
-    <cfRule type="expression" dxfId="3" priority="33">
+    <cfRule type="expression" dxfId="9" priority="41">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:EY14">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:EY20">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D26">
+  <conditionalFormatting sqref="I21:EY21 I24:EY28">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>AND(fin_tâche&gt;=L$5,début_tâche&lt;M$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{65AF7913-EB1B-40D4-849A-0899EEFC3B9A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:EY22">
+    <cfRule type="expression" dxfId="5" priority="8">
+      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:EY22">
+    <cfRule type="expression" dxfId="4" priority="7">
+      <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:EY22">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>AND(fin_tâche&gt;=L$5,début_tâche&lt;M$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -7249,12 +7681,22 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C8A27DA5-C50E-4041-867A-F6BB98AE46E8}</x14:id>
+          <x14:id>{9FB92A8B-BE3E-4BE3-AB9F-D846D5852014}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:EY26">
+  <conditionalFormatting sqref="I23:EY23">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23:EY23">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23:EY23">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(fin_tâche&gt;=L$5,début_tâche&lt;M$5)</formula>
     </cfRule>
@@ -7281,10 +7723,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D27:D28 D7:D21</xm:sqref>
+          <xm:sqref>D7:D21 D24:D30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C8A27DA5-C50E-4041-867A-F6BB98AE46E8}">
+          <x14:cfRule type="dataBar" id="{65AF7913-EB1B-40D4-849A-0899EEFC3B9A}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -7296,7 +7738,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D22:D26</xm:sqref>
+          <xm:sqref>D22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9FB92A8B-BE3E-4BE3-AB9F-D846D5852014}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>